<commit_message>
Decision final con TP y SL
</commit_message>
<xml_diff>
--- a/Programas e insumos/Insumos.xlsx
+++ b/Programas e insumos/Insumos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDSG\Wissen\GitHub\Swell_2_Optimizacion_estrategias\Programas e insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A385A732-BE1D-482C-9CD3-0FC667784221}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6704A020-1A83-445B-9157-389A28BDD38B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{59E37A4A-BA9D-486E-8155-2E7BBEED7B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Insumos" sheetId="2" r:id="rId1"/>
+    <sheet name="Zona_PG_Cierre" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Sortino_Objetivo</t>
   </si>
@@ -60,18 +61,9 @@
     <t>Informacion para cálculo de variables de riesgo</t>
   </si>
   <si>
-    <t>Cierre parcial menor</t>
-  </si>
-  <si>
-    <t>Cierre parcial mayor</t>
-  </si>
-  <si>
     <t>Comisión</t>
   </si>
   <si>
-    <t>Informacion de cierre y utilidad de negociación</t>
-  </si>
-  <si>
     <t>Apalancamiento máximo</t>
   </si>
   <si>
@@ -87,16 +79,34 @@
     <t>Informacion para filtro de datos</t>
   </si>
   <si>
-    <t>Take Profit Hard Limit (TPHL)</t>
-  </si>
-  <si>
-    <t>Take Profit Soft Limit (TPSL)</t>
-  </si>
-  <si>
-    <t>Stop Loss Hard Limit (SLHL)</t>
-  </si>
-  <si>
-    <t>Stop Loss Soft Limit (SLSL)</t>
+    <t>Cierre</t>
+  </si>
+  <si>
+    <t>Stop Loss</t>
+  </si>
+  <si>
+    <t>Low Loss</t>
+  </si>
+  <si>
+    <t>Low Profit</t>
+  </si>
+  <si>
+    <t>Take Profit</t>
+  </si>
+  <si>
+    <t>Bid-Ask Spread (BAS)</t>
+  </si>
+  <si>
+    <t>Informacion de negociación</t>
+  </si>
+  <si>
+    <t>Zona_PG</t>
+  </si>
+  <si>
+    <t>MinimoRazon</t>
+  </si>
+  <si>
+    <t>MaximoRazon</t>
   </si>
 </sst>
 </file>
@@ -107,7 +117,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,19 +140,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -168,16 +180,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,7 +517,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4873B9A-A335-448F-A0C1-E26E32A6A751}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -507,14 +530,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="3"/>
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>13</v>
@@ -522,156 +545,208 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3"/>
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3"/>
+      <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="6">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="4">
-        <v>1.4999999999999999E-2</v>
-      </c>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="4">
-        <v>2.5000000000000001E-2</v>
-      </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="4">
-        <v>0.5</v>
-      </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0.25</v>
+      <c r="A16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1">
-        <v>90</v>
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="4">
-        <v>0.05</v>
+      <c r="A20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="3"/>
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B24" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1">
         <v>0.4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E832472B-9A58-4630-968A-95C5F2276B14}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="8">
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>